<commit_message>
Started implementing the SQL database Structure into code and have now implemented the account screen adapter
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7891982A-C0B5-4848-95D7-003CE7D6A85C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EA40A26-51E1-4202-AE84-BF0828A30FDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,14 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Accounts</t>
   </si>
   <si>
-    <t>AccountId</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -66,9 +64,6 @@
     <t>Receipts</t>
   </si>
   <si>
-    <t>ReceiptId</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -123,16 +118,22 @@
     <t>Equal</t>
   </si>
   <si>
-    <t>Balances</t>
-  </si>
-  <si>
     <t>BalancesString</t>
   </si>
   <si>
-    <t>FK - AccountId</t>
-  </si>
-  <si>
     <t>Marie,£0.50,Dan</t>
+  </si>
+  <si>
+    <t>PK - ID</t>
+  </si>
+  <si>
+    <t>AccountUniqueId</t>
+  </si>
+  <si>
+    <t>Dan,£1,Teddylou/Marie,£2,Teddylou</t>
+  </si>
+  <si>
+    <t>ReceiptUniqueId</t>
   </si>
 </sst>
 </file>
@@ -490,173 +491,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="2">
-        <v>2.99</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
+      <c r="E13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SQL Database up and running, but needs certain input values from the itemized receipts, balances etc. Implemented Fragments in a tablayout pageViewAdapter
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EA40A26-51E1-4202-AE84-BF0828A30FDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32F059A0-666B-45D2-9F49-8B7C4AFC4C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Accounts</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>ReceiptUniqueId</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -173,10 +176,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,12 +510,12 @@
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -531,7 +535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -551,7 +555,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -571,12 +575,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -584,44 +588,50 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3">
+        <v>43982</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -638,7 +648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -655,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Enabled an easy date picker, enabled an easy currency picker, enabled each participants contribution to be retrieved and saved in the database
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32F059A0-666B-45D2-9F49-8B7C4AFC4C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037A26E3-3C39-4449-BFEF-5382172CEC18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
+    <workbookView xWindow="21120" yWindow="4836" windowWidth="2388" windowHeight="564" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Accounts</t>
   </si>
@@ -137,6 +136,12 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Contributions</t>
+  </si>
+  <si>
+    <t>Dan,£5/Marie,£5</t>
   </si>
 </sst>
 </file>
@@ -495,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,14 +513,15 @@
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -535,7 +541,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -555,7 +561,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -575,12 +581,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -600,10 +606,13 @@
         <v>11</v>
       </c>
       <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -622,16 +631,19 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -648,7 +660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -665,7 +677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Participants balances are now correctly impacted by each new expense. User can now add as many participants as they'd like. Many minor bugs have been fixed. I now need the functionaility available for the application to display to the user how the balances in a simple way
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037A26E3-3C39-4449-BFEF-5382172CEC18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1174D74C-4E9B-48DB-9A36-AB902003C150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21120" yWindow="4836" windowWidth="2388" windowHeight="564" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,18 +120,12 @@
     <t>BalancesString</t>
   </si>
   <si>
-    <t>Marie,£0.50,Dan</t>
-  </si>
-  <si>
     <t>PK - ID</t>
   </si>
   <si>
     <t>AccountUniqueId</t>
   </si>
   <si>
-    <t>Dan,£1,Teddylou/Marie,£2,Teddylou</t>
-  </si>
-  <si>
     <t>ReceiptUniqueId</t>
   </si>
   <si>
@@ -141,7 +135,13 @@
     <t>Contributions</t>
   </si>
   <si>
-    <t>Dan,£5/Marie,£5</t>
+    <t>Dan,£1,Dan/Marie,£1,Dan</t>
+  </si>
+  <si>
+    <t>Dan,3.00/Marie,-3.00</t>
+  </si>
+  <si>
+    <t>Dan,1.00/Marie,2.00/Teddylou,-3.00</t>
   </si>
 </sst>
 </file>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +513,7 @@
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -523,10 +523,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -558,7 +558,7 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -578,7 +578,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -588,13 +588,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -606,7 +606,7 @@
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
@@ -632,7 +632,7 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Created an algorithm described in Excel and implemented in ReceiptOverview.kt class. It is capable of working out an efficient way for eveybody to pay each other the money owed so that everyones balances can be settled. Steps have been commented throughout the algorithm explaining how.
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1174D74C-4E9B-48DB-9A36-AB902003C150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6B3311-5287-49C3-AFAB-8A76ED278369}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
+    <workbookView xWindow="17580" yWindow="3384" windowWidth="5256" windowHeight="5304" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Balance Sheet working" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
   <si>
     <t>Accounts</t>
   </si>
@@ -142,6 +143,120 @@
   </si>
   <si>
     <t>Dan,1.00/Marie,2.00/Teddylou,-3.00</t>
+  </si>
+  <si>
+    <t>rec00002</t>
+  </si>
+  <si>
+    <t>rec00003</t>
+  </si>
+  <si>
+    <t>First Expense</t>
+  </si>
+  <si>
+    <t>Second Expense</t>
+  </si>
+  <si>
+    <t>Dan,5.00,Dan/Dan,5.00,Marie/Dan,5.00,Tommy</t>
+  </si>
+  <si>
+    <t>Tommy</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Balance After Transaction</t>
+  </si>
+  <si>
+    <t>Dan,5.00,Dan/Marie,5.00,Dan/Tommy,5.00,Dan</t>
+  </si>
+  <si>
+    <t>Dan,5.00,Dan/Marie,5.00,Dan/Tommy,0.00,Dan</t>
+  </si>
+  <si>
+    <t>Positive List</t>
+  </si>
+  <si>
+    <t>marie</t>
+  </si>
+  <si>
+    <t>tommy</t>
+  </si>
+  <si>
+    <t>negative list</t>
+  </si>
+  <si>
+    <t>dan</t>
+  </si>
+  <si>
+    <t>Step 1: Separate into lists</t>
+  </si>
+  <si>
+    <t>Step 2: Largest negative balance?</t>
+  </si>
+  <si>
+    <t>Step 4: Is this less than the absolute value of the largest negative balance?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>no ---v</t>
+  </si>
+  <si>
+    <t>yes ---&gt;</t>
+  </si>
+  <si>
+    <t>Step 5(Yes): Take the absolute value of the largest negative from the largest positive.</t>
+  </si>
+  <si>
+    <t>Balance String</t>
+  </si>
+  <si>
+    <t>Dan,1,TeddyLou/Marie,2,TeddyLou</t>
+  </si>
+  <si>
+    <t>Largest Negative</t>
+  </si>
+  <si>
+    <t>Step 3: Largest Positive balance?</t>
+  </si>
+  <si>
+    <t>marie,10,dan</t>
+  </si>
+  <si>
+    <t>tommy,5,dan</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>repeat once</t>
+  </si>
+  <si>
+    <t>&lt;Scenario1) "Dan,-15.0/Marie,10.0/Tommy,5.0"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Largest Positive </t>
+  </si>
+  <si>
+    <t>Step 5(No): put the largest positive to the largest negative &amp; set string.</t>
+  </si>
+  <si>
+    <t>marie,9,dan</t>
+  </si>
+  <si>
+    <t>dan -6</t>
+  </si>
+  <si>
+    <t>&gt;Scenario2) "Dan,-15.0/Marie,-3.0/Tommy,18.0"</t>
+  </si>
+  <si>
+    <t>Step 6: Check if balanced and if not repeat process.</t>
+  </si>
+  <si>
+    <t>WhoOwesWho</t>
   </si>
 </sst>
 </file>
@@ -152,10 +267,29 @@
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,7 +303,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -177,15 +311,260 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,188 +892,672 @@
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="G2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="G4" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20">
+        <v>1</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="21">
+        <v>43982</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="22">
+        <v>10</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="20">
+        <v>1</v>
+      </c>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="20">
+        <v>2</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="21">
+        <v>43985</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="22">
+        <v>10</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C460858-8BFD-45A8-86E5-BC14F715AA34}">
+  <dimension ref="A7:P32"/>
+  <sheetViews>
+    <sheetView topLeftCell="H6" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28:O29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="11">
+        <v>43985</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="12">
+        <v>15</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="10">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3">
-        <v>43982</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="K9" s="10">
+        <v>-10</v>
+      </c>
+      <c r="L9" s="10">
+        <v>5</v>
+      </c>
+      <c r="M9" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="11">
+        <v>43985</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="12">
         <v>10</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8">
+      <c r="G10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2.99</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
+      <c r="K10" s="10">
+        <v>-5</v>
+      </c>
+      <c r="L10" s="10">
+        <v>5</v>
+      </c>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="4">
+        <f>SUM(K9:K10)</f>
+        <v>-15</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" ref="L12:M12" si="0">SUM(L9:L10)</f>
+        <v>10</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="O12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H15" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="25"/>
+      <c r="J15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H16" s="32"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="19" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H19" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="25"/>
+      <c r="J19" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K19" t="s">
+        <v>51</v>
+      </c>
+      <c r="M19" t="s">
+        <v>51</v>
+      </c>
+      <c r="N19" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H20" s="26"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="18">
+        <v>-15</v>
+      </c>
+      <c r="K20">
+        <v>-5</v>
+      </c>
+      <c r="M20">
+        <v>-15</v>
+      </c>
+      <c r="O20" s="23"/>
+    </row>
+    <row r="22" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H22" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="25"/>
+      <c r="J22" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" t="s">
+        <v>49</v>
+      </c>
+      <c r="M22" t="s">
+        <v>48</v>
+      </c>
+      <c r="O22" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="18">
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <v>5</v>
+      </c>
+      <c r="M23">
+        <v>9</v>
+      </c>
+      <c r="O23" s="23"/>
+    </row>
+    <row r="25" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H25" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="25"/>
+      <c r="J25" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="K25" t="s">
+        <v>55</v>
+      </c>
+      <c r="M25" t="s">
+        <v>55</v>
+      </c>
+      <c r="N25" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="O25" s="28"/>
+      <c r="P25" s="14"/>
+    </row>
+    <row r="26" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" t="s">
+        <v>55</v>
+      </c>
+      <c r="N26" s="26"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="18"/>
+    </row>
+    <row r="28" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H28" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" s="25"/>
+      <c r="J28" s="14"/>
+      <c r="K28" t="s">
+        <v>63</v>
+      </c>
+      <c r="M28" t="s">
+        <v>70</v>
+      </c>
+      <c r="N28" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="O28" s="25"/>
+      <c r="P28" s="14"/>
+    </row>
+    <row r="29" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H29" s="26"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="18"/>
+      <c r="K29" t="s">
+        <v>64</v>
+      </c>
+      <c r="N29" s="26"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="18"/>
+    </row>
+    <row r="31" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H31" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="25"/>
+      <c r="J31" s="14"/>
+      <c r="K31" t="s">
+        <v>66</v>
+      </c>
+      <c r="M31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H32" s="26"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="18"/>
+      <c r="K32" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="H31:I32"/>
+    <mergeCell ref="N25:O26"/>
+    <mergeCell ref="N28:O29"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="H15:I17"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="H22:I23"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="H28:I29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added an activity for an expense overview. Made a start on viewing the correct settlements. However at this time I have noticed my algorithm is not performing perfectly. It is to the dollar but not to the decimal point! Will look over this today
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6B3311-5287-49C3-AFAB-8A76ED278369}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03744EB6-8492-4940-87E9-B9C7846E940F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17580" yWindow="3384" windowWidth="5256" windowHeight="5304" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
   <si>
     <t>Accounts</t>
   </si>
@@ -256,7 +256,10 @@
     <t>Step 6: Check if balanced and if not repeat process.</t>
   </si>
   <si>
-    <t>WhoOwesWho</t>
+    <t>Settlements</t>
+  </si>
+  <si>
+    <t>SQL User (not in firebase)</t>
   </si>
 </sst>
 </file>
@@ -532,9 +535,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -563,6 +563,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -881,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -893,6 +896,7 @@
     <col min="4" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -931,7 +935,9 @@
       <c r="G2" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="20"/>
+      <c r="H2" s="20" t="s">
+        <v>75</v>
+      </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
     </row>
@@ -955,7 +961,9 @@
         <v>35</v>
       </c>
       <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="H3" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
     </row>
@@ -981,7 +989,9 @@
       <c r="G4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="20"/>
+      <c r="H4" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
     </row>
@@ -1225,13 +1235,13 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="30" t="s">
+      <c r="K7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="30" t="s">
+      <c r="L7" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="30" t="s">
+      <c r="M7" s="29" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1260,9 +1270,9 @@
       <c r="H8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
@@ -1363,10 +1373,10 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I15" s="25"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="13" t="s">
         <v>47</v>
       </c>
@@ -1375,8 +1385,8 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H16" s="32"/>
-      <c r="I16" s="33"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="32"/>
       <c r="J16" s="15" t="s">
         <v>48</v>
       </c>
@@ -1385,18 +1395,18 @@
       </c>
     </row>
     <row r="17" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H17" s="26"/>
-      <c r="I17" s="27"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="26"/>
       <c r="J17" s="17" t="s">
         <v>49</v>
       </c>
       <c r="K17" s="18"/>
     </row>
     <row r="19" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="I19" s="25"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="19" t="s">
         <v>51</v>
       </c>
@@ -1409,13 +1419,13 @@
       <c r="N19" t="s">
         <v>71</v>
       </c>
-      <c r="O19" s="23" t="s">
+      <c r="O19" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H20" s="26"/>
-      <c r="I20" s="27"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
       <c r="J20" s="18">
         <v>-15</v>
       </c>
@@ -1425,13 +1435,13 @@
       <c r="M20">
         <v>-15</v>
       </c>
-      <c r="O20" s="23"/>
+      <c r="O20" s="33"/>
     </row>
     <row r="22" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="I22" s="25"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="14" t="s">
         <v>48</v>
       </c>
@@ -1441,13 +1451,13 @@
       <c r="M22" t="s">
         <v>48</v>
       </c>
-      <c r="O22" s="23" t="s">
+      <c r="O22" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H23" s="26"/>
-      <c r="I23" s="27"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="26"/>
       <c r="J23" s="18">
         <v>10</v>
       </c>
@@ -1457,13 +1467,13 @@
       <c r="M23">
         <v>9</v>
       </c>
-      <c r="O23" s="23"/>
+      <c r="O23" s="33"/>
     </row>
     <row r="25" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H25" s="24" t="s">
+      <c r="H25" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="25"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="14" t="s">
         <v>57</v>
       </c>
@@ -1473,30 +1483,30 @@
       <c r="M25" t="s">
         <v>55</v>
       </c>
-      <c r="N25" s="24" t="s">
+      <c r="N25" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="O25" s="28"/>
+      <c r="O25" s="27"/>
       <c r="P25" s="14"/>
     </row>
     <row r="26" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H26" s="26"/>
-      <c r="I26" s="27"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="26"/>
       <c r="J26" s="18" t="s">
         <v>56</v>
       </c>
       <c r="K26" t="s">
         <v>55</v>
       </c>
-      <c r="N26" s="26"/>
-      <c r="O26" s="29"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="28"/>
       <c r="P26" s="18"/>
     </row>
     <row r="28" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H28" s="24" t="s">
+      <c r="H28" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="I28" s="25"/>
+      <c r="I28" s="24"/>
       <c r="J28" s="14"/>
       <c r="K28" t="s">
         <v>63</v>
@@ -1504,28 +1514,28 @@
       <c r="M28" t="s">
         <v>70</v>
       </c>
-      <c r="N28" s="24" t="s">
+      <c r="N28" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="O28" s="25"/>
+      <c r="O28" s="24"/>
       <c r="P28" s="14"/>
     </row>
     <row r="29" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H29" s="26"/>
-      <c r="I29" s="27"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26"/>
       <c r="J29" s="18"/>
       <c r="K29" t="s">
         <v>64</v>
       </c>
-      <c r="N29" s="26"/>
-      <c r="O29" s="27"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="26"/>
       <c r="P29" s="18"/>
     </row>
     <row r="31" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H31" s="24" t="s">
+      <c r="H31" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="I31" s="25"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="14"/>
       <c r="K31" t="s">
         <v>66</v>
@@ -1535,8 +1545,8 @@
       </c>
     </row>
     <row r="32" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H32" s="26"/>
-      <c r="I32" s="27"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="26"/>
       <c r="J32" s="18"/>
       <c r="K32" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Changed wording of accounts to groups from now on. Added ability to access an options activity for a group and within this to delete the entire group. Currently now looking to implement image selection and saving internally for the group profile icons
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03744EB6-8492-4940-87E9-B9C7846E940F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2E5DE2-5132-4099-8407-AF2F68489848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="3384" windowWidth="5256" windowHeight="5304" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
-  <si>
-    <t>Accounts</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -260,6 +257,12 @@
   </si>
   <si>
     <t>SQL User (not in firebase)</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>FK - GroupID</t>
   </si>
 </sst>
 </file>
@@ -884,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,7 +904,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -915,28 +918,28 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="C2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>2</v>
-      </c>
       <c r="E2" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>74</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>75</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
@@ -946,23 +949,23 @@
         <v>1</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
@@ -972,25 +975,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -1021,7 +1024,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -1035,28 +1038,28 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="D8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>33</v>
-      </c>
       <c r="H8" s="20" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
@@ -1066,22 +1069,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="21">
         <v>43982</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="22">
         <v>10</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="20">
         <v>1</v>
@@ -1094,22 +1097,22 @@
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="21">
         <v>43985</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="22">
         <v>10</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -1141,7 +1144,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -1155,19 +1158,19 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
         <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1175,13 +1178,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2">
         <v>2.99</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1192,13 +1195,13 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1233,42 +1236,42 @@
   <sheetData>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="H8" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -1279,22 +1282,22 @@
         <v>2</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="11">
         <v>43985</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="12">
         <v>15</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9" s="10">
         <v>1</v>
@@ -1314,22 +1317,22 @@
         <v>3</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="11">
         <v>43985</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="12">
         <v>10</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10" s="10">
         <v>1</v>
@@ -1344,12 +1347,12 @@
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J12" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K12" s="4">
         <f>SUM(K9:K10)</f>
@@ -1364,63 +1367,63 @@
         <v>5</v>
       </c>
       <c r="O12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H15" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I15" s="24"/>
       <c r="J15" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H16" s="31"/>
       <c r="I16" s="32"/>
       <c r="J16" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H17" s="25"/>
       <c r="I17" s="26"/>
       <c r="J17" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K17" s="18"/>
     </row>
     <row r="19" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H19" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O19" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="8:16" x14ac:dyDescent="0.3">
@@ -1439,20 +1442,20 @@
     </row>
     <row r="22" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H22" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I22" s="24"/>
       <c r="J22" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K22" t="s">
         <v>48</v>
       </c>
-      <c r="K22" t="s">
-        <v>49</v>
-      </c>
       <c r="M22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O22" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="8:16" x14ac:dyDescent="0.3">
@@ -1471,20 +1474,20 @@
     </row>
     <row r="25" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H25" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I25" s="24"/>
       <c r="J25" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" t="s">
+        <v>54</v>
+      </c>
+      <c r="M25" t="s">
+        <v>54</v>
+      </c>
+      <c r="N25" s="23" t="s">
         <v>57</v>
-      </c>
-      <c r="K25" t="s">
-        <v>55</v>
-      </c>
-      <c r="M25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N25" s="23" t="s">
-        <v>58</v>
       </c>
       <c r="O25" s="27"/>
       <c r="P25" s="14"/>
@@ -1493,10 +1496,10 @@
       <c r="H26" s="25"/>
       <c r="I26" s="26"/>
       <c r="J26" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N26" s="25"/>
       <c r="O26" s="28"/>
@@ -1504,18 +1507,18 @@
     </row>
     <row r="28" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H28" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I28" s="24"/>
       <c r="J28" s="14"/>
       <c r="K28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N28" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O28" s="24"/>
       <c r="P28" s="14"/>
@@ -1525,7 +1528,7 @@
       <c r="I29" s="26"/>
       <c r="J29" s="18"/>
       <c r="K29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N29" s="25"/>
       <c r="O29" s="26"/>
@@ -1533,15 +1536,15 @@
     </row>
     <row r="31" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H31" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I31" s="24"/>
       <c r="J31" s="14"/>
       <c r="K31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="8:16" x14ac:dyDescent="0.3">
@@ -1549,7 +1552,7 @@
       <c r="I32" s="26"/>
       <c r="J32" s="18"/>
       <c r="K32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI for scanned receipt items working with horizontal scroll view and radio groups for every participant. Backend created to convert the itemized products into contribution strings ready to update the balances and settlement amounts
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2E5DE2-5132-4099-8407-AF2F68489848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BAAF8E-28FE-4E81-B9DC-223809FA3366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Strawberries</t>
   </si>
   <si>
-    <t>For Whome</t>
-  </si>
-  <si>
     <t>Tea</t>
   </si>
   <si>
@@ -263,6 +260,12 @@
   </si>
   <si>
     <t>FK - GroupID</t>
+  </si>
+  <si>
+    <t>Ownership</t>
+  </si>
+  <si>
+    <t>Scanned</t>
   </si>
 </sst>
 </file>
@@ -885,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,9 +905,9 @@
     <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -916,12 +919,12 @@
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>29</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -933,18 +936,18 @@
         <v>13</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>74</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -961,7 +964,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
@@ -970,7 +973,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>2</v>
       </c>
@@ -987,10 +990,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>12</v>
@@ -998,7 +1001,7 @@
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -1010,7 +1013,7 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -1022,7 +1025,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>8</v>
       </c>
@@ -1036,15 +1039,15 @@
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>31</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>16</v>
@@ -1056,15 +1059,18 @@
         <v>10</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="20"/>
+        <v>77</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>75</v>
+      </c>
       <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>1</v>
       </c>
@@ -1084,26 +1090,29 @@
         <v>12</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="20">
+        <v>32</v>
+      </c>
+      <c r="H9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="20">
         <v>1</v>
       </c>
-      <c r="I9" s="20"/>
       <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="21">
         <v>43985</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="22">
         <v>10</v>
@@ -1112,13 +1121,18 @@
         <v>12</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+        <v>39</v>
+      </c>
+      <c r="H10" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="20">
+        <v>2</v>
+      </c>
       <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="21"/>
@@ -1130,7 +1144,7 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -1142,7 +1156,7 @@
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>19</v>
       </c>
@@ -1156,9 +1170,9 @@
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -1167,13 +1181,13 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1190,18 +1204,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1242,21 +1256,21 @@
         <v>12</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>16</v>
@@ -1268,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>11</v>
@@ -1282,13 +1296,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="11">
         <v>43985</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="12">
         <v>15</v>
@@ -1297,7 +1311,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="10">
         <v>1</v>
@@ -1317,13 +1331,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="11">
         <v>43985</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="12">
         <v>10</v>
@@ -1332,7 +1346,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H10" s="10">
         <v>1</v>
@@ -1347,12 +1361,12 @@
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J12" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K12" s="4">
         <f>SUM(K9:K10)</f>
@@ -1367,63 +1381,63 @@
         <v>5</v>
       </c>
       <c r="O12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H15" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" s="24"/>
       <c r="J15" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H16" s="31"/>
       <c r="I16" s="32"/>
       <c r="J16" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H17" s="25"/>
       <c r="I17" s="26"/>
       <c r="J17" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K17" s="18"/>
     </row>
     <row r="19" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H19" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O19" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="8:16" x14ac:dyDescent="0.3">
@@ -1442,20 +1456,20 @@
     </row>
     <row r="22" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H22" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I22" s="24"/>
       <c r="J22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" t="s">
         <v>47</v>
       </c>
-      <c r="K22" t="s">
-        <v>48</v>
-      </c>
       <c r="M22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O22" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="8:16" x14ac:dyDescent="0.3">
@@ -1474,20 +1488,20 @@
     </row>
     <row r="25" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H25" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I25" s="24"/>
       <c r="J25" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K25" t="s">
+        <v>53</v>
+      </c>
+      <c r="M25" t="s">
+        <v>53</v>
+      </c>
+      <c r="N25" s="23" t="s">
         <v>56</v>
-      </c>
-      <c r="K25" t="s">
-        <v>54</v>
-      </c>
-      <c r="M25" t="s">
-        <v>54</v>
-      </c>
-      <c r="N25" s="23" t="s">
-        <v>57</v>
       </c>
       <c r="O25" s="27"/>
       <c r="P25" s="14"/>
@@ -1496,10 +1510,10 @@
       <c r="H26" s="25"/>
       <c r="I26" s="26"/>
       <c r="J26" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N26" s="25"/>
       <c r="O26" s="28"/>
@@ -1507,18 +1521,18 @@
     </row>
     <row r="28" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H28" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I28" s="24"/>
       <c r="J28" s="14"/>
       <c r="K28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N28" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O28" s="24"/>
       <c r="P28" s="14"/>
@@ -1528,7 +1542,7 @@
       <c r="I29" s="26"/>
       <c r="J29" s="18"/>
       <c r="K29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N29" s="25"/>
       <c r="O29" s="26"/>
@@ -1536,15 +1550,15 @@
     </row>
     <row r="31" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H31" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I31" s="24"/>
       <c r="J31" s="14"/>
       <c r="K31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="8:16" x14ac:dyDescent="0.3">
@@ -1552,7 +1566,7 @@
       <c r="I32" s="26"/>
       <c r="J32" s="18"/>
       <c r="K32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Consolidated sql functions into helper class. Began creating helper class for firebase db. Decided on using timestamps for now to ensure new groups and expenses are unique. Also refactored large parts of the code for clarity. Expenses are now any new transaction entered and receipt will refer only to scanned receipts
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BAAF8E-28FE-4E81-B9DC-223809FA3366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5147217-2B46-4F51-A4C3-2E0080EF0096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>Scanned</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>ExpenseUniqueId</t>
   </si>
 </sst>
 </file>
@@ -891,7 +897,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,7 +1033,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -1044,7 +1050,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Added ability that each user sync any updates when they sign in to a group. Also fixed a few minor bugs throughout the app.
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5147217-2B46-4F51-A4C3-2E0080EF0096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1031B8C1-703E-4269-BEF3-8DCE8A79C31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -40,18 +40,12 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Pbhbdy46218</t>
-  </si>
-  <si>
     <t>HouseShare</t>
   </si>
   <si>
     <t>House</t>
   </si>
   <si>
-    <t>57Gfsgdkji</t>
-  </si>
-  <si>
     <t>Trip</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>PK - ID</t>
   </si>
   <si>
-    <t>AccountUniqueId</t>
-  </si>
-  <si>
     <t>ReceiptUniqueId</t>
   </si>
   <si>
@@ -272,6 +263,12 @@
   </si>
   <si>
     <t>ExpenseUniqueId</t>
+  </si>
+  <si>
+    <t>FirebaseId</t>
+  </si>
+  <si>
+    <t>LastEdit</t>
   </si>
 </sst>
 </file>
@@ -897,7 +894,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,7 +910,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -927,10 +924,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -939,72 +936,78 @@
         <v>1</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="20"/>
+        <v>70</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>78</v>
+      </c>
       <c r="J2" s="20"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="20">
+        <v>161515166</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>4</v>
-      </c>
       <c r="E3" s="20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="20"/>
+        <v>10</v>
+      </c>
+      <c r="I3" s="20">
+        <v>56465464</v>
+      </c>
       <c r="J3" s="20"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="20">
+        <v>211615351</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="20"/>
+        <v>10</v>
+      </c>
+      <c r="I4" s="20">
+        <v>56151561</v>
+      </c>
       <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1033,7 +1036,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -1047,31 +1050,31 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="D8" s="20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
@@ -1081,22 +1084,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="21">
         <v>43982</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="22">
         <v>10</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H9" s="20" t="b">
         <v>0</v>
@@ -1112,22 +1115,22 @@
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" s="21">
         <v>43985</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E10" s="22">
         <v>10</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H10" s="20" t="b">
         <v>1</v>
@@ -1164,7 +1167,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -1178,19 +1181,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
         <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1198,13 +1201,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2">
         <v>2.99</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1215,13 +1218,13 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1256,42 +1259,42 @@
   <sheetData>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="D8" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>11</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -1302,22 +1305,22 @@
         <v>2</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9" s="11">
         <v>43985</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="12">
         <v>15</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H9" s="10">
         <v>1</v>
@@ -1337,22 +1340,22 @@
         <v>3</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" s="11">
         <v>43985</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E10" s="12">
         <v>10</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H10" s="10">
         <v>1</v>
@@ -1367,12 +1370,12 @@
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J12" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K12" s="4">
         <f>SUM(K9:K10)</f>
@@ -1387,63 +1390,63 @@
         <v>5</v>
       </c>
       <c r="O12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H15" s="23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I15" s="24"/>
       <c r="J15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="K15" s="14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H16" s="31"/>
       <c r="I16" s="32"/>
       <c r="J16" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="16" t="s">
         <v>46</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H17" s="25"/>
       <c r="I17" s="26"/>
       <c r="J17" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K17" s="18"/>
     </row>
     <row r="19" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H19" s="23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O19" s="33" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="8:16" x14ac:dyDescent="0.3">
@@ -1462,20 +1465,20 @@
     </row>
     <row r="22" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H22" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I22" s="24"/>
       <c r="J22" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O22" s="33" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="8:16" x14ac:dyDescent="0.3">
@@ -1494,20 +1497,20 @@
     </row>
     <row r="25" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H25" s="23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I25" s="24"/>
       <c r="J25" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K25" t="s">
+        <v>50</v>
+      </c>
+      <c r="M25" t="s">
+        <v>50</v>
+      </c>
+      <c r="N25" s="23" t="s">
         <v>53</v>
-      </c>
-      <c r="M25" t="s">
-        <v>53</v>
-      </c>
-      <c r="N25" s="23" t="s">
-        <v>56</v>
       </c>
       <c r="O25" s="27"/>
       <c r="P25" s="14"/>
@@ -1516,10 +1519,10 @@
       <c r="H26" s="25"/>
       <c r="I26" s="26"/>
       <c r="J26" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N26" s="25"/>
       <c r="O26" s="28"/>
@@ -1527,18 +1530,18 @@
     </row>
     <row r="28" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H28" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I28" s="24"/>
       <c r="J28" s="14"/>
       <c r="K28" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M28" t="s">
+        <v>65</v>
+      </c>
+      <c r="N28" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="N28" s="23" t="s">
-        <v>71</v>
       </c>
       <c r="O28" s="24"/>
       <c r="P28" s="14"/>
@@ -1548,7 +1551,7 @@
       <c r="I29" s="26"/>
       <c r="J29" s="18"/>
       <c r="K29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N29" s="25"/>
       <c r="O29" s="26"/>
@@ -1556,15 +1559,15 @@
     </row>
     <row r="31" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H31" s="23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I31" s="24"/>
       <c r="J31" s="14"/>
       <c r="K31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="8:16" x14ac:dyDescent="0.3">
@@ -1572,7 +1575,7 @@
       <c r="I32" s="26"/>
       <c r="J32" s="18"/>
       <c r="K32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to upload and download group profile images as and when members of the group change the image
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1031B8C1-703E-4269-BEF3-8DCE8A79C31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD627D90-DA2F-4CB8-B30A-9B90D35CDC2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>LastEdit</t>
+  </si>
+  <si>
+    <t>LastImageEdit</t>
   </si>
 </sst>
 </file>
@@ -906,6 +909,7 @@
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -948,7 +952,7 @@
         <v>70</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J2" s="20"/>
     </row>
@@ -976,7 +980,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="20">
-        <v>56465464</v>
+        <v>551561551</v>
       </c>
       <c r="J3" s="20"/>
     </row>
@@ -1006,7 +1010,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="20">
-        <v>56151561</v>
+        <v>645656454</v>
       </c>
       <c r="J4" s="20"/>
     </row>
@@ -1019,7 +1023,6 @@
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
       <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1031,7 +1034,6 @@
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
       <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1045,7 +1047,6 @@
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
       <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1074,9 +1075,11 @@
         <v>74</v>
       </c>
       <c r="I8" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="J8" s="20"/>
       <c r="K8" s="20"/>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1105,9 +1108,11 @@
         <v>0</v>
       </c>
       <c r="I9" s="20">
+        <v>56465464</v>
+      </c>
+      <c r="J9" s="20">
         <v>1</v>
       </c>
-      <c r="J9" s="20"/>
       <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1136,9 +1141,11 @@
         <v>1</v>
       </c>
       <c r="I10" s="20">
+        <v>56151561</v>
+      </c>
+      <c r="J10" s="20">
         <v>2</v>
       </c>
-      <c r="J10" s="20"/>
       <c r="K10" s="20"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed some minor bugs, updated db schemas for both fb and sql
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD627D90-DA2F-4CB8-B30A-9B90D35CDC2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E72D8AA-6C64-4B40-9B37-CED8A38CA874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SQL Structure" sheetId="1" r:id="rId1"/>
     <sheet name="Balance Sheet working" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -160,87 +160,27 @@
     <t>Dan,5.00,Dan/Marie,5.00,Dan/Tommy,0.00,Dan</t>
   </si>
   <si>
-    <t>Positive List</t>
-  </si>
-  <si>
     <t>marie</t>
   </si>
   <si>
-    <t>tommy</t>
-  </si>
-  <si>
-    <t>negative list</t>
-  </si>
-  <si>
     <t>dan</t>
   </si>
   <si>
-    <t>Step 1: Separate into lists</t>
-  </si>
-  <si>
-    <t>Step 2: Largest negative balance?</t>
-  </si>
-  <si>
-    <t>Step 4: Is this less than the absolute value of the largest negative balance?</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>no ---v</t>
   </si>
   <si>
     <t>yes ---&gt;</t>
   </si>
   <si>
-    <t>Step 5(Yes): Take the absolute value of the largest negative from the largest positive.</t>
-  </si>
-  <si>
-    <t>Balance String</t>
-  </si>
-  <si>
     <t>Dan,1,TeddyLou/Marie,2,TeddyLou</t>
   </si>
   <si>
     <t>Largest Negative</t>
   </si>
   <si>
-    <t>Step 3: Largest Positive balance?</t>
-  </si>
-  <si>
-    <t>marie,10,dan</t>
-  </si>
-  <si>
-    <t>tommy,5,dan</t>
-  </si>
-  <si>
-    <t>finished</t>
-  </si>
-  <si>
-    <t>repeat once</t>
-  </si>
-  <si>
-    <t>&lt;Scenario1) "Dan,-15.0/Marie,10.0/Tommy,5.0"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Largest Positive </t>
   </si>
   <si>
-    <t>Step 5(No): put the largest positive to the largest negative &amp; set string.</t>
-  </si>
-  <si>
-    <t>marie,9,dan</t>
-  </si>
-  <si>
-    <t>dan -6</t>
-  </si>
-  <si>
-    <t>&gt;Scenario2) "Dan,-15.0/Marie,-3.0/Tommy,18.0"</t>
-  </si>
-  <si>
-    <t>Step 6: Check if balanced and if not repeat process.</t>
-  </si>
-  <si>
     <t>Settlements</t>
   </si>
   <si>
@@ -272,6 +212,54 @@
   </si>
   <si>
     <t>LastImageEdit</t>
+  </si>
+  <si>
+    <t>Step 1: Largest negative balance?</t>
+  </si>
+  <si>
+    <t>Step 2: Largest Positive balance?</t>
+  </si>
+  <si>
+    <t>Step 3: Is this less than the absolute value of the largest negative balance?</t>
+  </si>
+  <si>
+    <t>Step 4(No): put the largest positive to the largest negative &amp; set string.</t>
+  </si>
+  <si>
+    <t>Step 5: Check if balanced and if not repeat process.</t>
+  </si>
+  <si>
+    <t>Step 4(Yes): Take the absolute value of the largest negative from the largest positive.</t>
+  </si>
+  <si>
+    <t>GroupCurrency</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>ExpenseCurrency</t>
+  </si>
+  <si>
+    <t>UiSymbol</t>
+  </si>
+  <si>
+    <t>£</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>ExpenseExchangeRate</t>
+  </si>
+  <si>
+    <t>A$</t>
   </si>
 </sst>
 </file>
@@ -318,7 +306,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -499,29 +487,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -535,11 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -569,12 +535,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -894,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,281 +872,323 @@
     <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16">
+        <v>161515166</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="16">
+        <v>551561551</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+    </row>
+    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16">
+        <v>211615351</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="16">
+        <v>645656454</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="B8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="16"/>
+    </row>
+    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="17">
+        <v>43982</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="18">
+        <v>10</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="I9" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="16">
         <v>1</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20">
+      <c r="L9" s="16">
+        <v>56465464</v>
+      </c>
+      <c r="M9" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="20">
-        <v>161515166</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="N9" s="16"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
         <v>2</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="B10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="17">
+        <v>43985</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="18">
         <v>10</v>
       </c>
-      <c r="I3" s="20">
-        <v>551561551</v>
-      </c>
-      <c r="J3" s="20"/>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20">
+      <c r="F10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="16">
+        <v>1.5309999999999999</v>
+      </c>
+      <c r="L10" s="16">
+        <v>56151561</v>
+      </c>
+      <c r="M10" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="20">
-        <v>211615351</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="20">
-        <v>645656454</v>
-      </c>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="J5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
-        <v>1</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="21">
-        <v>43982</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="22">
-        <v>10</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="20">
-        <v>56465464</v>
-      </c>
-      <c r="J9" s="20">
-        <v>1</v>
-      </c>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="20">
-        <v>2</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="21">
-        <v>43985</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="22">
-        <v>10</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="20">
-        <v>56151561</v>
-      </c>
-      <c r="J10" s="20">
-        <v>2</v>
-      </c>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="N10" s="16"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1197,13 +1199,13 @@
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1220,7 +1222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1246,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C460858-8BFD-45A8-86E5-BC14F715AA34}">
-  <dimension ref="A7:P32"/>
+  <dimension ref="A7:P28"/>
   <sheetViews>
-    <sheetView topLeftCell="H6" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28:O29"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1268,13 +1270,13 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="29" t="s">
+      <c r="L7" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="29" t="s">
+      <c r="M7" s="25" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1303,9 +1305,9 @@
       <c r="H8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
@@ -1375,11 +1377,7 @@
       </c>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="O11" t="s">
-        <v>54</v>
-      </c>
-    </row>
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J12" s="6" t="s">
         <v>39</v>
@@ -1396,210 +1394,117 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="O12" t="s">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H15" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="20"/>
+      <c r="J15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="O15" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H16" s="21"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="14">
+        <v>-15</v>
+      </c>
+      <c r="O16" s="27"/>
+    </row>
+    <row r="18" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H18" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="20"/>
+      <c r="J18" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H19" s="21"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="14">
+        <v>10</v>
+      </c>
+      <c r="O19" s="27"/>
+    </row>
+    <row r="21" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H21" s="19" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H15" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="K15" s="14" t="s">
+      <c r="I21" s="20"/>
+      <c r="J21" s="13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H16" s="31"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H17" s="25"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="17" t="s">
+      <c r="N21" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="O21" s="23"/>
+      <c r="P21" s="13"/>
+    </row>
+    <row r="22" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H22" s="21"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="K17" s="18"/>
-    </row>
-    <row r="19" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H19" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="K19" t="s">
-        <v>46</v>
-      </c>
-      <c r="M19" t="s">
-        <v>46</v>
-      </c>
-      <c r="N19" t="s">
-        <v>66</v>
-      </c>
-      <c r="O19" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="18">
-        <v>-15</v>
-      </c>
-      <c r="K20">
-        <v>-5</v>
-      </c>
-      <c r="M20">
-        <v>-15</v>
-      </c>
-      <c r="O20" s="33"/>
-    </row>
-    <row r="22" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H22" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="I22" s="24"/>
-      <c r="J22" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="K22" t="s">
-        <v>44</v>
-      </c>
-      <c r="M22" t="s">
-        <v>43</v>
-      </c>
-      <c r="O22" s="33" t="s">
+      <c r="N22" s="21"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="14"/>
+    </row>
+    <row r="24" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H24" s="19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H23" s="25"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="18">
-        <v>10</v>
-      </c>
-      <c r="K23">
-        <v>5</v>
-      </c>
-      <c r="M23">
-        <v>9</v>
-      </c>
-      <c r="O23" s="33"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="13"/>
+      <c r="N24" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="O24" s="20"/>
+      <c r="P24" s="13"/>
     </row>
     <row r="25" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H25" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="I25" s="24"/>
-      <c r="J25" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K25" t="s">
-        <v>50</v>
-      </c>
-      <c r="M25" t="s">
-        <v>50</v>
-      </c>
-      <c r="N25" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="O25" s="27"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="14"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="22"/>
       <c r="P25" s="14"/>
     </row>
-    <row r="26" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H26" s="25"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="K26" t="s">
-        <v>50</v>
-      </c>
-      <c r="N26" s="25"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="18"/>
+    <row r="27" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H27" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I27" s="20"/>
+      <c r="J27" s="13"/>
     </row>
     <row r="28" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="I28" s="24"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="22"/>
       <c r="J28" s="14"/>
-      <c r="K28" t="s">
-        <v>58</v>
-      </c>
-      <c r="M28" t="s">
-        <v>65</v>
-      </c>
-      <c r="N28" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="O28" s="24"/>
-      <c r="P28" s="14"/>
-    </row>
-    <row r="29" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H29" s="25"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="18"/>
-      <c r="K29" t="s">
-        <v>59</v>
-      </c>
-      <c r="N29" s="25"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="18"/>
-    </row>
-    <row r="31" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H31" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="I31" s="24"/>
-      <c r="J31" s="14"/>
-      <c r="K31" t="s">
-        <v>61</v>
-      </c>
-      <c r="M31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H32" s="25"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="18"/>
-      <c r="K32" t="s">
-        <v>60</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="H31:I32"/>
-    <mergeCell ref="N25:O26"/>
-    <mergeCell ref="N28:O29"/>
+  <mergeCells count="12">
+    <mergeCell ref="H27:I28"/>
+    <mergeCell ref="N21:O22"/>
+    <mergeCell ref="N24:O25"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
-    <mergeCell ref="H15:I17"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="H22:I23"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="H28:I29"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="H18:I19"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="H24:I25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Re-structured how participants names and balances are stored. New SQL table, new Firebase DB structure, new methods to add participants into a group and retrieve new participants from DB when they are not stored in SQL due to another user being added
</commit_message>
<xml_diff>
--- a/Workings/SqlDataBaseStructureDraft.xlsx
+++ b/Workings/SqlDataBaseStructureDraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan96\Documents\SplitReceiptApp\Workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E72D8AA-6C64-4B40-9B37-CED8A38CA874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030242B8-E9FE-4070-B6E4-BF5EBD33396E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F371CC5-43FF-4E86-BFEB-41EE8CAB8B14}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -67,15 +67,6 @@
     <t>Dan</t>
   </si>
   <si>
-    <t>Participants</t>
-  </si>
-  <si>
-    <t>Dan, Marie</t>
-  </si>
-  <si>
-    <t>Dan, Marie, Teddylou</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -106,9 +97,6 @@
     <t>Equal</t>
   </si>
   <si>
-    <t>BalancesString</t>
-  </si>
-  <si>
     <t>PK - ID</t>
   </si>
   <si>
@@ -124,12 +112,6 @@
     <t>Dan,£1,Dan/Marie,£1,Dan</t>
   </si>
   <si>
-    <t>Dan,3.00/Marie,-3.00</t>
-  </si>
-  <si>
-    <t>Dan,1.00/Marie,2.00/Teddylou,-3.00</t>
-  </si>
-  <si>
     <t>rec00002</t>
   </si>
   <si>
@@ -260,6 +242,42 @@
   </si>
   <si>
     <t>A$</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>FBaseUniqueID</t>
+  </si>
+  <si>
+    <t>Uname</t>
+  </si>
+  <si>
+    <t>Ubalance</t>
+  </si>
+  <si>
+    <t>Dan125</t>
+  </si>
+  <si>
+    <t>ParticipantsLastEdit</t>
+  </si>
+  <si>
+    <t>Dan,1,Marie</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>LastUpdate</t>
   </si>
 </sst>
 </file>
@@ -854,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB916-4769-4E69-BF70-D451ED521994}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,14 +885,14 @@
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
     <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -888,10 +906,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>0</v>
@@ -900,25 +918,22 @@
         <v>1</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -934,24 +949,23 @@
       <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>12</v>
+      <c r="E3" s="16">
+        <v>15847725</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="16">
+      <c r="H3" s="16">
         <v>551561551</v>
       </c>
+      <c r="I3" s="16" t="s">
+        <v>61</v>
+      </c>
       <c r="J3" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -967,26 +981,23 @@
       <c r="D4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>13</v>
+      <c r="E4" s="16">
+        <v>15558585</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="16">
+      <c r="H4" s="16">
         <v>645656454</v>
       </c>
+      <c r="I4" s="16" t="s">
+        <v>62</v>
+      </c>
       <c r="J4" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1013,7 +1024,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -1026,16 +1037,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>7</v>
@@ -1044,25 +1055,25 @@
         <v>8</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N8" s="16"/>
     </row>
@@ -1071,13 +1082,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="17">
         <v>43982</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E9" s="18">
         <v>10</v>
@@ -1086,16 +1097,16 @@
         <v>10</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H9" s="16" t="b">
         <v>0</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K9" s="16">
         <v>1</v>
@@ -1113,13 +1124,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C10" s="17">
         <v>43985</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E10" s="18">
         <v>10</v>
@@ -1128,16 +1139,16 @@
         <v>10</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H10" s="16" t="b">
         <v>1</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="K10" s="16">
         <v>1.5309999999999999</v>
@@ -1176,7 +1187,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1190,19 +1201,19 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1210,7 +1221,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2">
         <v>2.99</v>
@@ -1227,15 +1238,93 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21">
+        <v>1.7</v>
+      </c>
+      <c r="E21">
+        <v>155145465</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
         <v>1</v>
       </c>
     </row>
@@ -1274,24 +1363,24 @@
         <v>10</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="M7" s="25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>7</v>
@@ -1300,7 +1389,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>9</v>
@@ -1314,13 +1403,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C9" s="11">
         <v>43985</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E9" s="12">
         <v>15</v>
@@ -1329,7 +1418,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H9" s="10">
         <v>1</v>
@@ -1349,13 +1438,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C10" s="11">
         <v>43985</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E10" s="12">
         <v>10</v>
@@ -1364,7 +1453,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H10" s="10">
         <v>1</v>
@@ -1380,7 +1469,7 @@
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J12" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K12" s="4">
         <f>SUM(K9:K10)</f>
@@ -1397,14 +1486,14 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H15" s="19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I15" s="20"/>
       <c r="J15" s="15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -1417,14 +1506,14 @@
     </row>
     <row r="18" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H18" s="19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I18" s="20"/>
       <c r="J18" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O18" s="27" t="s">
         <v>42</v>
-      </c>
-      <c r="O18" s="27" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="8:16" x14ac:dyDescent="0.3">
@@ -1437,14 +1526,14 @@
     </row>
     <row r="21" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H21" s="19" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I21" s="20"/>
       <c r="J21" s="13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="O21" s="23"/>
       <c r="P21" s="13"/>
@@ -1453,7 +1542,7 @@
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
       <c r="J22" s="14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="N22" s="21"/>
       <c r="O22" s="24"/>
@@ -1461,12 +1550,12 @@
     </row>
     <row r="24" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H24" s="19" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I24" s="20"/>
       <c r="J24" s="13"/>
       <c r="N24" s="19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="O24" s="20"/>
       <c r="P24" s="13"/>
@@ -1481,7 +1570,7 @@
     </row>
     <row r="27" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H27" s="19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I27" s="20"/>
       <c r="J27" s="13"/>

</xml_diff>